<commit_message>
Practise SUM, MIN/MAX, AVERAGE, COUNT, AutoSum and adjacent cells error.
</commit_message>
<xml_diff>
--- a/excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
+++ b/excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8FE122016AAF1840/Belgeler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{5CBF3812-D25A-4E09-A2D9-642B56D4155B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EB89025-701A-4A5D-A41A-4F8EC1A23F1A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F685894C-4DBB-491C-A033-AF17F621D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{4EC8B933-5C16-44B8-8BD1-3B03B4E7E629}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Montlhy Budget</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -70,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -114,7 +126,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -132,10 +144,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC8743-1258-4C1E-92E6-82DF26842A77}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,11 +587,11 @@
         <v>950</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" ref="E5:E9" si="0">SUM(B5:D5)</f>
         <v>2900</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F9" si="0">E5/$E$9</f>
+        <f t="shared" ref="F5:F9" si="1">E5/$E$9</f>
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
@@ -601,11 +609,11 @@
         <v>1400</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>4400</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
@@ -623,11 +631,11 @@
         <v>24000</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>68000</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
     </row>
@@ -645,11 +653,11 @@
         <v>5350</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>16700</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3500000000000005E-2</v>
       </c>
     </row>
@@ -658,27 +666,115 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>B4+B5+B6+B7+B8</f>
+        <f>SUM(B4:B8)</f>
         <v>78000</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:D9" si="1">C4+C5+C6+C7+C8</f>
+        <f t="shared" ref="C9:D9" si="2">SUM(C4:C8)</f>
         <v>55300</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>66700</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>66700</v>
-      </c>
-      <c r="E9">
-        <f>SUM(B9:D9)</f>
-        <v>200000</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>MIN(B4:B8)</f>
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <f>MIN(C4:C8)</f>
+        <v>950</v>
+      </c>
+      <c r="D11">
+        <f>MIN(D4:D8)</f>
+        <v>950</v>
+      </c>
+      <c r="E11">
+        <f>MIN(E4:E8)</f>
+        <v>2900</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>MAX(B4:B8)</f>
+        <v>48000</v>
+      </c>
+      <c r="C12">
+        <f>MAX(C4:C8)</f>
+        <v>25000</v>
+      </c>
+      <c r="D12">
+        <f>MAX(D4:D8)</f>
+        <v>35000</v>
+      </c>
+      <c r="E12">
+        <f>MAX(E4:E8)</f>
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B4:B8)</f>
+        <v>15600</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C4:C8)</f>
+        <v>11060</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D4:D8)</f>
+        <v>13340</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E4:E8)</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B4:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f>COUNT(C4:C8)</f>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f>COUNT(D4:D8)</f>
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f>COUNT(E4:E8)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B13:D14 B9:D9 B11:D12" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update budget sheet formatting and calculations.
</commit_message>
<xml_diff>
--- a/excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
+++ b/excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F685894C-4DBB-491C-A033-AF17F621D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66C3143-7455-4654-9DD3-1E9FE2D9AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{4EC8B933-5C16-44B8-8BD1-3B03B4E7E629}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Monthly Budget " sheetId="12" r:id="rId1"/>
+    <sheet name="Copy Exercise" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Montlhy Budget</t>
   </si>
@@ -75,16 +76,22 @@
   </si>
   <si>
     <t>COUNT</t>
+  </si>
+  <si>
+    <t>Online Shopping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,16 +108,59 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,22 +168,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="AwesomeStyle" xfId="3" xr:uid="{65150C0F-7736-4FBF-89DC-FF58D6DB8DAA}"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -463,7 +590,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -512,24 +639,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC8743-1258-4C1E-92E6-82DF26842A77}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD3905B-E95B-4636-863D-328414AE3C59}">
+  <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="37.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <v>45292</v>
+      </c>
+      <c r="D5" s="11">
+        <v>45323</v>
+      </c>
+      <c r="E5" s="11">
+        <v>45717</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>48000</v>
+      </c>
+      <c r="D6" s="5">
+        <v>25000</v>
+      </c>
+      <c r="E6" s="5">
+        <v>35000</v>
+      </c>
+      <c r="F6" s="6">
+        <f>SUM(C6:E6)</f>
+        <v>108000</v>
+      </c>
+      <c r="G6" s="8">
+        <f>F6/$F$12</f>
+        <v>0.52735919997656178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="7">
+        <v>950</v>
+      </c>
+      <c r="E7" s="7">
+        <v>950</v>
+      </c>
+      <c r="F7" s="7">
+        <f>SUM(C7:E7)</f>
+        <v>2900</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" ref="G7:G12" si="0">F7/$F$12</f>
+        <v>1.4160571110481752E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7">
+        <v>350</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4324</v>
+      </c>
+      <c r="E8" s="7">
+        <v>120</v>
+      </c>
+      <c r="F8" s="7">
+        <f>SUM(C8:E8)</f>
+        <v>4794</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.340888893229294E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1500</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1500</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1400</v>
+      </c>
+      <c r="F9" s="7">
+        <f>SUM(C9:E9)</f>
+        <v>4400</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1485004443489556E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
+        <v>22000</v>
+      </c>
+      <c r="D10" s="7">
+        <v>22000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>24000</v>
+      </c>
+      <c r="F10" s="7">
+        <f>SUM(C10:E10)</f>
+        <v>68000</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.33204097776302038</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5500</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5850</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5350</v>
+      </c>
+      <c r="F11" s="7">
+        <f>SUM(C11:E11)</f>
+        <v>16700</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>8.1545357774153546E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <f>SUM(C6:C11)</f>
+        <v>78350</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12:E12" si="1">SUM(D6:D11)</f>
+        <v>59624</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>66820</v>
+      </c>
+      <c r="F12" s="6">
+        <f>SUM(C12:E12)</f>
+        <v>204794</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f>MIN(C6:C11)</f>
+        <v>350</v>
+      </c>
+      <c r="D14">
+        <f>MIN(D6:D11)</f>
+        <v>950</v>
+      </c>
+      <c r="E14">
+        <f>MIN(E6:E11)</f>
+        <v>120</v>
+      </c>
+      <c r="F14" s="4">
+        <f>MIN(F6:F11)</f>
+        <v>2900</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f>MAX(C6:C11)</f>
+        <v>48000</v>
+      </c>
+      <c r="D15">
+        <f>MAX(D6:D11)</f>
+        <v>25000</v>
+      </c>
+      <c r="E15">
+        <f>MAX(E6:E11)</f>
+        <v>35000</v>
+      </c>
+      <c r="F15" s="4">
+        <f>MAX(F6:F11)</f>
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <f>AVERAGE(C6:C11)</f>
+        <v>13058.333333333334</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(D6:D11)</f>
+        <v>9937.3333333333339</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(E6:E11)</f>
+        <v>11136.666666666666</v>
+      </c>
+      <c r="F16" s="4">
+        <f>AVERAGE(F6:F11)</f>
+        <v>34132.333333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4">
+        <f>COUNT(C6:C11)</f>
+        <v>6</v>
+      </c>
+      <c r="D17" s="4">
+        <f>COUNT(D6:D11)</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="4">
+        <f>COUNT(E6:E11)</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="4">
+        <f>COUNT(F6:F11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C6:E11">
+    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C14:E17 C12:E12" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63FC743-2487-47E6-ADBA-53D754771889}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -544,7 +982,7 @@
       <c r="D3" s="2">
         <v>45717</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -564,217 +1002,239 @@
       <c r="D4">
         <v>35000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <f>SUM(B4:D4)</f>
         <v>108000</v>
       </c>
-      <c r="F4" s="3">
-        <f>E4/$E$9</f>
-        <v>0.54</v>
+      <c r="F4" s="3" t="e">
+        <f>E4/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>1000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>950</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>950</v>
       </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E9" si="0">SUM(B5:D5)</f>
+      <c r="E5" s="4">
+        <f>SUM(B5:D5)</f>
         <v>2900</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" ref="F5:F9" si="1">E5/$E$9</f>
-        <v>1.4500000000000001E-2</v>
+      <c r="F5" s="3" t="e">
+        <f>E5/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1500</v>
-      </c>
-      <c r="C6">
-        <v>1500</v>
-      </c>
-      <c r="D6">
-        <v>1400</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>4400</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" si="1"/>
-        <v>2.1999999999999999E-2</v>
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>350</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4324</v>
+      </c>
+      <c r="D6" s="4">
+        <v>120</v>
+      </c>
+      <c r="E6" s="4">
+        <f>SUM(B6:D6)</f>
+        <v>4794</v>
+      </c>
+      <c r="F6" s="3" t="e">
+        <f>E6/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>22000</v>
+        <v>1500</v>
       </c>
       <c r="C7">
-        <v>22000</v>
+        <v>1500</v>
       </c>
       <c r="D7">
-        <v>24000</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>68000</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.34</v>
+        <v>1400</v>
+      </c>
+      <c r="E7" s="4">
+        <f>SUM(B7:D7)</f>
+        <v>4400</v>
+      </c>
+      <c r="F7" s="3" t="e">
+        <f>E7/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>5500</v>
+        <v>22000</v>
       </c>
       <c r="C8">
-        <v>5850</v>
+        <v>22000</v>
       </c>
       <c r="D8">
-        <v>5350</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>16700</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="1"/>
-        <v>8.3500000000000005E-2</v>
+        <v>24000</v>
+      </c>
+      <c r="E8" s="4">
+        <f>SUM(B8:D8)</f>
+        <v>68000</v>
+      </c>
+      <c r="F8" s="3" t="e">
+        <f>E8/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>5500</v>
+      </c>
+      <c r="C9">
+        <v>5850</v>
+      </c>
+      <c r="D9">
+        <v>5350</v>
+      </c>
+      <c r="E9" s="4">
+        <f>SUM(B9:D9)</f>
+        <v>16700</v>
+      </c>
+      <c r="F9" s="3" t="e">
+        <f>E9/$F$12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <f>SUM(B4:B8)</f>
-        <v>78000</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:D9" si="2">SUM(C4:C8)</f>
-        <v>55300</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>66700</v>
-      </c>
-      <c r="E9">
+      <c r="B10">
+        <f>SUM(B4:B9)</f>
+        <v>78350</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D10" si="0">SUM(C4:C9)</f>
+        <v>59624</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>200000</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>66820</v>
+      </c>
+      <c r="E10" s="4">
+        <f>SUM(B10:D10)</f>
+        <v>204794</v>
+      </c>
+      <c r="F10" s="3" t="e">
+        <f>E10/$F$12</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <f>MIN(B4:B8)</f>
-        <v>1000</v>
-      </c>
-      <c r="C11">
-        <f>MIN(C4:C8)</f>
-        <v>950</v>
-      </c>
-      <c r="D11">
-        <f>MIN(D4:D8)</f>
-        <v>950</v>
-      </c>
-      <c r="E11">
-        <f>MIN(E4:E8)</f>
-        <v>2900</v>
-      </c>
-      <c r="F11" s="3"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <f>MAX(B4:B8)</f>
-        <v>48000</v>
+        <f>MIN(B4:B9)</f>
+        <v>350</v>
       </c>
       <c r="C12">
-        <f>MAX(C4:C8)</f>
-        <v>25000</v>
+        <f>MIN(C4:C9)</f>
+        <v>950</v>
       </c>
       <c r="D12">
-        <f>MAX(D4:D8)</f>
-        <v>35000</v>
-      </c>
-      <c r="E12">
-        <f>MAX(E4:E8)</f>
-        <v>108000</v>
-      </c>
+        <f>MIN(D4:D9)</f>
+        <v>120</v>
+      </c>
+      <c r="E12" s="4">
+        <f>MIN(E4:E9)</f>
+        <v>2900</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <f>AVERAGE(B4:B8)</f>
-        <v>15600</v>
+        <f>MAX(B4:B9)</f>
+        <v>48000</v>
       </c>
       <c r="C13">
-        <f>AVERAGE(C4:C8)</f>
-        <v>11060</v>
+        <f>MAX(C4:C9)</f>
+        <v>25000</v>
       </c>
       <c r="D13">
-        <f>AVERAGE(D4:D8)</f>
-        <v>13340</v>
-      </c>
-      <c r="E13">
-        <f>AVERAGE(E4:E8)</f>
-        <v>40000</v>
+        <f>MAX(D4:D9)</f>
+        <v>35000</v>
+      </c>
+      <c r="E13" s="4">
+        <f>MAX(E4:E9)</f>
+        <v>108000</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B4:B9)</f>
+        <v>13058.333333333334</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C4:C9)</f>
+        <v>9937.3333333333339</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(D4:D9)</f>
+        <v>11136.666666666666</v>
+      </c>
+      <c r="E14" s="4">
+        <f>AVERAGE(E4:E9)</f>
+        <v>34132.333333333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <f>COUNT(B4:B8)</f>
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <f>COUNT(C4:C8)</f>
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <f>COUNT(D4:D8)</f>
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <f>COUNT(E4:E8)</f>
-        <v>5</v>
+      <c r="B15">
+        <f>COUNT(B4:B9)</f>
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>COUNT(C4:C9)</f>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f>COUNT(D4:D9)</f>
+        <v>6</v>
+      </c>
+      <c r="E15" s="4">
+        <f>COUNT(E4:E9)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B13:D14 B9:D9 B11:D12" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>